<commit_message>
Added some new JUnit Tests
</commit_message>
<xml_diff>
--- a/Test Plan/Test Traker.xlsx
+++ b/Test Plan/Test Traker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12015" yWindow="1440" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12015" yWindow="1440" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="201">
   <si>
     <t>Test ID</t>
   </si>
@@ -622,6 +622,12 @@
   </si>
   <si>
     <t>"Cancel" click</t>
+  </si>
+  <si>
+    <t>testDeleteStlFile</t>
+  </si>
+  <si>
+    <t>PG1</t>
   </si>
 </sst>
 </file>
@@ -928,6 +934,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -937,13 +950,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -963,7 +969,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C107" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C107" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C107"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Test ID" dataDxfId="2"/>
@@ -1298,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1325,15 +1331,23 @@
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1747,15 +1761,23 @@
       <c r="A44" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
+      <c r="B44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
+      <c r="B45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -1993,7 +2015,7 @@
         <v>85</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>154</v>
@@ -2001,10 +2023,14 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -2385,7 +2411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test Tracker - Moved Integration and Verification tests to Manual Tests
</commit_message>
<xml_diff>
--- a/Test Plan/Test Traker.xlsx
+++ b/Test Plan/Test Traker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12015" yWindow="1440" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="12015" yWindow="1440" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="206">
   <si>
     <t>Test ID</t>
   </si>
@@ -628,6 +628,21 @@
   </si>
   <si>
     <t>PG1</t>
+  </si>
+  <si>
+    <t>SG1</t>
+  </si>
+  <si>
+    <t>Button presses, Text input</t>
+  </si>
+  <si>
+    <t>Displays are updated and menus switch correctly</t>
+  </si>
+  <si>
+    <t>Filenames</t>
+  </si>
+  <si>
+    <t>Controllers save/load configurations correctly</t>
   </si>
 </sst>
 </file>
@@ -677,7 +692,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -796,6 +811,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -826,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -844,6 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -969,8 +996,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C107" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C100" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C100"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Test ID" dataDxfId="2"/>
     <tableColumn id="2" name="Test Name" dataDxfId="1"/>
@@ -1302,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1877,24 +1904,32 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>93</v>
@@ -1902,10 +1937,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>93</v>
@@ -1913,10 +1948,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>93</v>
@@ -1924,10 +1959,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>93</v>
@@ -1935,10 +1970,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>93</v>
@@ -1946,10 +1981,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>93</v>
@@ -1957,10 +1992,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>93</v>
@@ -1968,10 +2003,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>93</v>
@@ -1979,10 +2014,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>93</v>
@@ -1990,140 +2025,160 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>93</v>
+        <v>156</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>93</v>
+        <v>158</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>154</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>154</v>
+      <c r="A72" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="3"/>
+      <c r="A73" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="3"/>
+      <c r="A74" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="3"/>
+      <c r="A75" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="3"/>
+      <c r="A76" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B77" s="1"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="12" t="s">
+      <c r="A79" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C80" s="12" t="s">
+      <c r="A80" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" s="12" t="s">
+      <c r="A81" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C82" s="12" t="s">
+      <c r="A82" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>114</v>
+      <c r="A83" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>93</v>
@@ -2131,87 +2186,87 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>123</v>
+      <c r="A85" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>124</v>
+      <c r="A86" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>125</v>
+      <c r="A87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>121</v>
+      <c r="A88" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>121</v>
+      <c r="A89" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>130</v>
+      <c r="A90" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C90" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>137</v>
+      <c r="A91" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>93</v>
@@ -2222,7 +2277,7 @@
         <v>84</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C92" s="15" t="s">
         <v>93</v>
@@ -2233,18 +2288,18 @@
         <v>84</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>141</v>
+      <c r="A94" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>93</v>
@@ -2252,10 +2307,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>93</v>
@@ -2263,10 +2318,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>93</v>
@@ -2274,10 +2329,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>93</v>
@@ -2285,111 +2340,34 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>93</v>
+      <c r="A99" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
+      <c r="A100" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B107" s="8" t="s">
+      <c r="B100" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C100" s="9" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2409,18 +2387,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="5" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="41.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="25.125" customWidth="1"/>
   </cols>
@@ -2848,6 +2826,81 @@
         <v>174</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
* Added tests to manual tests
</commit_message>
<xml_diff>
--- a/Test Plan/Test Traker.xlsx
+++ b/Test Plan/Test Traker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SRDesign\Test Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\SRDesign\Test Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="232">
   <si>
     <t>Test ID</t>
   </si>
@@ -643,6 +643,84 @@
   </si>
   <si>
     <t>Controllers save/load configurations correctly</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>G-Code file. UI "Cancel"</t>
+  </si>
+  <si>
+    <t>G-Code stream is halted</t>
+  </si>
+  <si>
+    <t>Printer status exits thread terminating G-Code stream</t>
+  </si>
+  <si>
+    <t>G-Code file. Temperature feedback</t>
+  </si>
+  <si>
+    <t>Printer status hangs in loop waiting for temps to fall</t>
+  </si>
+  <si>
+    <t>Printer status hangs in loop waiting for resume when paused</t>
+  </si>
+  <si>
+    <t>G-Code file. UI "Pause/Resume"</t>
+  </si>
+  <si>
+    <t>Printer feedback data</t>
+  </si>
+  <si>
+    <t>Temperature data populated in TemperatureObject</t>
+  </si>
+  <si>
+    <t>TemperatureObject correctly populated with tool temps</t>
+  </si>
+  <si>
+    <t>G-Code file</t>
+  </si>
+  <si>
+    <t>Serialize g-codes with correct line endings</t>
+  </si>
+  <si>
+    <t>G-codes have correct line endings, comments are stripped</t>
+  </si>
+  <si>
+    <t>Feedback information correctly stored and assembled</t>
+  </si>
+  <si>
+    <t>PrintJobConfiguration obj</t>
+  </si>
+  <si>
+    <t>Successfully connect to printer</t>
+  </si>
+  <si>
+    <t>Successfully connected to printer. Fails otherwise</t>
+  </si>
+  <si>
+    <t>Serialized G-code</t>
+  </si>
+  <si>
+    <t>Successfully poll and send G-code to printer</t>
+  </si>
+  <si>
+    <t>Module successfully sends serialized G-Codes to printer</t>
+  </si>
+  <si>
+    <t>Successfully read printer feedback data when ready</t>
+  </si>
+  <si>
+    <t>Printer feedback string is successfully read</t>
+  </si>
+  <si>
+    <t>G-Code File. PrintJobConfiguration Object. Printer Feedback data</t>
+  </si>
+  <si>
+    <t>Est. Connection to printer, send g-codes and populate feedback object</t>
+  </si>
+  <si>
+    <t>Connection established, g-codes send successfully and feedback data populated</t>
   </si>
 </sst>
 </file>
@@ -961,13 +1039,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -977,6 +1048,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -996,8 +1074,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C100" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C90" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C90"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Test ID" dataDxfId="2"/>
     <tableColumn id="2" name="Test Name" dataDxfId="1"/>
@@ -1329,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1841,73 +1919,109 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>93</v>
@@ -1915,10 +2029,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>93</v>
@@ -1926,259 +2040,263 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>93</v>
+        <v>156</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>77</v>
+        <v>200</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>93</v>
+        <v>158</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>128</v>
+      <c r="A62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>131</v>
+      <c r="A63" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>133</v>
+      <c r="A64" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>134</v>
+      <c r="A65" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C66" s="12" t="s">
+      <c r="A66" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" s="12" t="s">
+      <c r="A67" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="12" t="s">
+      <c r="B75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>114</v>
+      <c r="A76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>122</v>
+      <c r="A77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>123</v>
+      <c r="A78" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>124</v>
+      <c r="A79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>125</v>
+      <c r="A80" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>121</v>
+      <c r="A81" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>121</v>
+      <c r="A82" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>130</v>
+      <c r="A83" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>93</v>
@@ -2189,7 +2307,7 @@
         <v>129</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>93</v>
@@ -2197,10 +2315,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>93</v>
@@ -2208,10 +2326,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>93</v>
@@ -2219,10 +2337,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>93</v>
@@ -2230,144 +2348,34 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>93</v>
+      <c r="A89" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
+      <c r="A90" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B100" s="8" t="s">
+      <c r="B90" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C90" s="9" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2387,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2901,6 +2909,206 @@
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" t="s">
+        <v>208</v>
+      </c>
+      <c r="E29" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" t="s">
+        <v>208</v>
+      </c>
+      <c r="E30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" t="s">
+        <v>214</v>
+      </c>
+      <c r="D32" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" t="s">
+        <v>218</v>
+      </c>
+      <c r="E33" t="s">
+        <v>219</v>
+      </c>
+      <c r="F33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" t="s">
+        <v>226</v>
+      </c>
+      <c r="F36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E37" t="s">
+        <v>228</v>
+      </c>
+      <c r="F37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>